<commit_message>
pulled needed census data and exported to csv, updated dataset columns
</commit_message>
<xml_diff>
--- a/project-scrapbook.xlsx
+++ b/project-scrapbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisamarieth/projects/covid-19_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B801558-3EBB-6F4F-8DE9-9EF6969A4DBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF03005A-E008-A54E-9709-4D48D94FD75E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43700" yWindow="8480" windowWidth="39180" windowHeight="20380" xr2:uid="{90358BCF-BB8A-A94A-9E76-B4B6749AEB0E}"/>
+    <workbookView xWindow="41700" yWindow="7500" windowWidth="39180" windowHeight="20380" xr2:uid="{90358BCF-BB8A-A94A-9E76-B4B6749AEB0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>week #</t>
   </si>
@@ -107,9 +107,6 @@
     <t>deaths_since_01212020</t>
   </si>
   <si>
-    <t>days_until_plateau</t>
-  </si>
-  <si>
     <t>implemented_stay_at_home</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>y (state level)</t>
   </si>
   <si>
-    <t>tbc (int)</t>
-  </si>
-  <si>
     <t>tbc (boolean)</t>
   </si>
   <si>
@@ -138,6 +132,15 @@
   </si>
   <si>
     <t>%_pop_commuting_public_transport</t>
+  </si>
+  <si>
+    <t>y (boolean)</t>
+  </si>
+  <si>
+    <t>at_least_100pct_w2w3_dec</t>
+  </si>
+  <si>
+    <t>less_than_25pct_wow_inc</t>
   </si>
 </sst>
 </file>
@@ -165,12 +168,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -200,14 +209,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5939CBF3-A53F-0648-A1A4-D2A6D29101F3}">
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -544,20 +555,20 @@
     <col min="12" max="12" width="20.1640625" customWidth="1"/>
     <col min="13" max="13" width="20.83203125" customWidth="1"/>
     <col min="14" max="14" width="17.33203125" customWidth="1"/>
-    <col min="15" max="15" width="26" customWidth="1"/>
+    <col min="15" max="15" width="22.83203125" customWidth="1"/>
     <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="19.83203125" customWidth="1"/>
     <col min="20" max="20" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D1" t="s">
@@ -569,88 +580,94 @@
       <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>21</v>
       </c>
       <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="Q2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+    </row>
+    <row r="7" spans="1:17">
       <c r="C7" t="s">
         <v>0</v>
       </c>
@@ -658,7 +675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>0</v>
       </c>
@@ -674,7 +691,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>1</v>
       </c>
@@ -690,7 +707,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>2</v>
       </c>
@@ -706,7 +723,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>3</v>
       </c>
@@ -722,7 +739,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>4</v>
       </c>
@@ -738,7 +755,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>5</v>
       </c>
@@ -754,7 +771,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>6</v>
       </c>
@@ -770,7 +787,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>7</v>
       </c>
@@ -783,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>8</v>
       </c>
@@ -967,32 +984,32 @@
       <c r="C34">
         <v>754</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J34" s="3"/>
-      <c r="L34" s="3" t="s">
+      <c r="J34" s="2"/>
+      <c r="L34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M34" s="3" t="s">
+      <c r="M34" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N34" s="3" t="s">
+      <c r="N34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O34" s="3" t="s">
+      <c r="O34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P34" s="3" t="s">
+      <c r="P34" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1006,35 +1023,35 @@
       <c r="C35">
         <v>345</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H35" s="3">
-        <v>1</v>
-      </c>
-      <c r="I35" s="3">
+      <c r="H35" s="2">
+        <v>1</v>
+      </c>
+      <c r="I35" s="2">
         <v>13</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="3">
         <f xml:space="preserve"> 22 - 13</f>
         <v>9</v>
       </c>
-      <c r="L35" s="3" t="s">
+      <c r="L35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M35" s="3" t="s">
+      <c r="M35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N35" s="3">
-        <v>1</v>
-      </c>
-      <c r="O35" s="3">
+      <c r="N35" s="2">
+        <v>1</v>
+      </c>
+      <c r="O35" s="2">
         <v>12</v>
       </c>
-      <c r="P35" s="3">
+      <c r="P35" s="2">
         <f>AVERAGE(O35:O41)</f>
         <v>13.428571428571429</v>
       </c>
@@ -1049,75 +1066,75 @@
       <c r="C36">
         <v>23</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3">
-        <v>2</v>
-      </c>
-      <c r="I36" s="3">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2">
+        <v>2</v>
+      </c>
+      <c r="I36" s="2">
         <v>22</v>
       </c>
-      <c r="J36" s="5">
+      <c r="J36" s="4">
         <f>9/13</f>
         <v>0.69230769230769229</v>
       </c>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3">
-        <v>1</v>
-      </c>
-      <c r="O36" s="3">
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2">
+        <v>1</v>
+      </c>
+      <c r="O36" s="2">
         <v>12</v>
       </c>
-      <c r="P36" s="3"/>
+      <c r="P36" s="2"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3">
-        <v>3</v>
-      </c>
-      <c r="I37" s="3">
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2">
+        <v>3</v>
+      </c>
+      <c r="I37" s="2">
         <v>30</v>
       </c>
-      <c r="J37" s="6">
+      <c r="J37" s="5">
         <f>0.69*100</f>
         <v>69</v>
       </c>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3">
-        <v>1</v>
-      </c>
-      <c r="O37" s="3">
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2">
+        <v>1</v>
+      </c>
+      <c r="O37" s="2">
         <v>12</v>
       </c>
-      <c r="P37" s="3"/>
+      <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>6</v>
       </c>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3">
-        <v>1</v>
-      </c>
-      <c r="O38" s="3">
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2">
+        <v>1</v>
+      </c>
+      <c r="O38" s="2">
         <v>12</v>
       </c>
-      <c r="P38" s="3"/>
+      <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16">
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3">
-        <v>1</v>
-      </c>
-      <c r="O39" s="3">
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2">
+        <v>1</v>
+      </c>
+      <c r="O39" s="2">
         <v>12</v>
       </c>
-      <c r="P39" s="3"/>
+      <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16">
       <c r="A40" t="s">
@@ -1129,229 +1146,229 @@
       <c r="C40" t="s">
         <v>5</v>
       </c>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3">
-        <v>1</v>
-      </c>
-      <c r="O40" s="3">
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2">
+        <v>1</v>
+      </c>
+      <c r="O40" s="2">
         <v>17</v>
       </c>
-      <c r="P40" s="3"/>
+      <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16">
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H41" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="I41" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J41" s="3" t="s">
+      <c r="J41" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3">
-        <v>1</v>
-      </c>
-      <c r="O41" s="3">
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2">
+        <v>1</v>
+      </c>
+      <c r="O41" s="2">
         <v>17</v>
       </c>
-      <c r="P41" s="3"/>
+      <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16">
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H42" s="3">
-        <v>1</v>
-      </c>
-      <c r="I42" s="3">
-        <v>2</v>
-      </c>
-      <c r="J42" s="3">
+      <c r="H42" s="2">
+        <v>1</v>
+      </c>
+      <c r="I42" s="2">
+        <v>2</v>
+      </c>
+      <c r="J42" s="2">
         <f>((I36 - I35) / ABS(I35)) * 100</f>
         <v>69.230769230769226</v>
       </c>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3">
-        <v>2</v>
-      </c>
-      <c r="O42" s="3">
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2">
+        <v>2</v>
+      </c>
+      <c r="O42" s="2">
         <v>19</v>
       </c>
-      <c r="P42" s="3">
+      <c r="P42" s="2">
         <f>AVERAGE(O42:O48)</f>
         <v>22.285714285714285</v>
       </c>
     </row>
     <row r="43" spans="1:16">
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3">
-        <v>2</v>
-      </c>
-      <c r="I43" s="3">
-        <v>3</v>
-      </c>
-      <c r="J43" s="3">
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2">
+        <v>2</v>
+      </c>
+      <c r="I43" s="2">
+        <v>3</v>
+      </c>
+      <c r="J43" s="2">
         <f>((I37 - I36) / ABS(I36)) * 100</f>
         <v>36.363636363636367</v>
       </c>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3">
-        <v>2</v>
-      </c>
-      <c r="O43" s="3">
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2">
+        <v>2</v>
+      </c>
+      <c r="O43" s="2">
         <v>19</v>
       </c>
-      <c r="P43" s="3"/>
+      <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16">
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3">
-        <v>2</v>
-      </c>
-      <c r="O44" s="3">
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2">
+        <v>2</v>
+      </c>
+      <c r="O44" s="2">
         <v>19</v>
       </c>
-      <c r="P44" s="3"/>
+      <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16">
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3">
-        <v>2</v>
-      </c>
-      <c r="O45" s="3">
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2">
+        <v>2</v>
+      </c>
+      <c r="O45" s="2">
         <v>23</v>
       </c>
-      <c r="P45" s="3"/>
+      <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16">
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3">
-        <v>2</v>
-      </c>
-      <c r="O46" s="3">
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2">
+        <v>2</v>
+      </c>
+      <c r="O46" s="2">
         <v>25</v>
       </c>
-      <c r="P46" s="3"/>
+      <c r="P46" s="2"/>
     </row>
     <row r="47" spans="1:16">
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3">
-        <v>2</v>
-      </c>
-      <c r="O47" s="3">
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2">
+        <v>2</v>
+      </c>
+      <c r="O47" s="2">
         <v>25</v>
       </c>
-      <c r="P47" s="3"/>
+      <c r="P47" s="2"/>
     </row>
     <row r="48" spans="1:16">
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3">
-        <v>2</v>
-      </c>
-      <c r="O48" s="3">
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2">
+        <v>2</v>
+      </c>
+      <c r="O48" s="2">
         <v>26</v>
       </c>
-      <c r="P48" s="3"/>
+      <c r="P48" s="2"/>
     </row>
     <row r="49" spans="12:16">
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3">
-        <v>3</v>
-      </c>
-      <c r="O49" s="3">
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2">
+        <v>3</v>
+      </c>
+      <c r="O49" s="2">
         <v>25</v>
       </c>
-      <c r="P49" s="3">
+      <c r="P49" s="2">
         <f>AVERAGE(O49:O55)</f>
         <v>30.142857142857142</v>
       </c>
     </row>
     <row r="50" spans="12:16">
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3">
-        <v>3</v>
-      </c>
-      <c r="O50" s="3">
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2">
+        <v>3</v>
+      </c>
+      <c r="O50" s="2">
         <v>27</v>
       </c>
-      <c r="P50" s="3"/>
+      <c r="P50" s="2"/>
     </row>
     <row r="51" spans="12:16">
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3">
-        <v>3</v>
-      </c>
-      <c r="O51" s="3">
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2">
+        <v>3</v>
+      </c>
+      <c r="O51" s="2">
         <v>28</v>
       </c>
-      <c r="P51" s="3"/>
+      <c r="P51" s="2"/>
     </row>
     <row r="52" spans="12:16">
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3">
-        <v>3</v>
-      </c>
-      <c r="O52" s="3">
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2">
+        <v>3</v>
+      </c>
+      <c r="O52" s="2">
         <v>30</v>
       </c>
-      <c r="P52" s="3"/>
+      <c r="P52" s="2"/>
     </row>
     <row r="53" spans="12:16">
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3">
-        <v>3</v>
-      </c>
-      <c r="O53" s="3">
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2">
+        <v>3</v>
+      </c>
+      <c r="O53" s="2">
         <v>32</v>
       </c>
-      <c r="P53" s="3"/>
+      <c r="P53" s="2"/>
     </row>
     <row r="54" spans="12:16">
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3">
-        <v>3</v>
-      </c>
-      <c r="O54" s="3">
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2">
+        <v>3</v>
+      </c>
+      <c r="O54" s="2">
         <v>33</v>
       </c>
-      <c r="P54" s="3"/>
+      <c r="P54" s="2"/>
     </row>
     <row r="55" spans="12:16">
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3">
-        <v>3</v>
-      </c>
-      <c r="O55" s="3">
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2">
+        <v>3</v>
+      </c>
+      <c r="O55" s="2">
         <v>36</v>
       </c>
-      <c r="P55" s="3"/>
+      <c r="P55" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cleaned up and built datasets needed, converted csvs to arff format
</commit_message>
<xml_diff>
--- a/project-scrapbook.xlsx
+++ b/project-scrapbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisamarieth/projects/covid-19_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8871CB66-4825-B144-A575-5EB04D84F829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DC723C-30A2-6C40-A56F-92883E56BF34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="23560" xr2:uid="{90358BCF-BB8A-A94A-9E76-B4B6749AEB0E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="35">
   <si>
     <t>week #</t>
   </si>
@@ -107,9 +107,6 @@
     <t>deaths_since_01212020</t>
   </si>
   <si>
-    <t>implemented_stay_at_home</t>
-  </si>
-  <si>
     <t>high_chance_of_death</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>y (state level)</t>
   </si>
   <si>
-    <t>tbc (boolean)</t>
-  </si>
-  <si>
     <t>%_pop_over_65</t>
   </si>
   <si>
@@ -141,6 +135,9 @@
   </si>
   <si>
     <t>less_than_25pct_wow_inc</t>
+  </si>
+  <si>
+    <t>imposed_intervention</t>
   </si>
 </sst>
 </file>
@@ -209,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -217,7 +214,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -537,27 +533,27 @@
   <dimension ref="A1:Q55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="23.5" customWidth="1"/>
-    <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" customWidth="1"/>
-    <col min="11" max="11" width="31.5" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" customWidth="1"/>
-    <col min="13" max="13" width="20.83203125" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" customWidth="1"/>
-    <col min="15" max="15" width="22.83203125" customWidth="1"/>
-    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.83203125" customWidth="1"/>
     <col min="20" max="20" width="10.83203125" customWidth="1"/>
   </cols>
@@ -581,91 +577,138 @@
       <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>27</v>
-      </c>
       <c r="Q2" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:17">

</xml_diff>